<commit_message>
fix description and priority
</commit_message>
<xml_diff>
--- a/MetroLondres/output/xlsx/Calculo do menor trajeto entre duas estações--GT-.xlsx
+++ b/MetroLondres/output/xlsx/Calculo do menor trajeto entre duas estações--GT-.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlhel\workspace\Trajetos_Metro_Londres\MetroLondres\output\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="7305"/>
   </bookViews>
@@ -10,12 +15,11 @@
     <sheet name="Test Suite" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <oleSize ref="A1:L16"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="86">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -249,6 +253,30 @@
   </si>
   <si>
     <t>dasdas</t>
+  </si>
+  <si>
+    <t>Testar fluxo completo</t>
+  </si>
+  <si>
+    <t>Testar nomes das estações 1</t>
+  </si>
+  <si>
+    <t>Testar nomes das estações 2</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Testar nomes das estações 3</t>
+  </si>
+  <si>
+    <t>Testar nomes das estações 4</t>
+  </si>
+  <si>
+    <t>Testar nomes das estações 5</t>
   </si>
 </sst>
 </file>
@@ -424,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -453,15 +481,6 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -479,6 +498,24 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,10 +852,10 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="19" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -831,8 +868,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
@@ -843,13 +878,13 @@
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
+      <c r="D6" s="21" t="s">
+        <v>82</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="14" t="s">
         <v>61</v>
       </c>
     </row>
@@ -857,19 +892,19 @@
       <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="11" t="s">
+      <c r="B7" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="13">
         <v>44112</v>
       </c>
     </row>
@@ -877,19 +912,19 @@
       <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="C8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>2</v>
       </c>
     </row>
@@ -926,7 +961,7 @@
       <c r="D10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="10" t="s">
         <v>55</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -940,13 +975,13 @@
       <c r="B11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="10" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="10" t="s">
         <v>55</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -960,20 +995,19 @@
       <c r="B12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="10" t="s">
         <v>52</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>4</v>
@@ -981,13 +1015,13 @@
       <c r="B14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="10" t="s">
         <v>53</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="10" t="s">
         <v>55</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -1001,20 +1035,19 @@
       <c r="B15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="10" t="s">
         <v>57</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>6</v>
@@ -1028,7 +1061,7 @@
       <c r="D17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="10" t="s">
         <v>55</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -1042,13 +1075,13 @@
       <c r="B18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="10" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="10" t="s">
         <v>55</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -1068,7 +1101,7 @@
       <c r="D19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="10" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -1079,24 +1112,22 @@
       <c r="A20" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25"/>
+      <c r="C20" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>12</v>
@@ -1107,13 +1138,13 @@
       <c r="C23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>2</v>
+      <c r="D23" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="14" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1121,19 +1152,19 @@
       <c r="A24" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="11" t="s">
+      <c r="B24" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="13">
         <v>44112</v>
       </c>
     </row>
@@ -1141,19 +1172,19 @@
       <c r="A25" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" s="12" t="s">
+      <c r="C25" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="17" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1190,7 +1221,7 @@
       <c r="D27" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="10" t="s">
         <v>55</v>
       </c>
       <c r="F27" s="5" t="s">
@@ -1204,20 +1235,19 @@
       <c r="B28" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="10" t="s">
         <v>56</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>3</v>
@@ -1225,20 +1255,19 @@
       <c r="B30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>4</v>
@@ -1246,13 +1275,13 @@
       <c r="B32" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F32" s="5" t="s">
@@ -1266,21 +1295,19 @@
       <c r="B33" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="12">
         <v>-2</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>6</v>
@@ -1288,21 +1315,19 @@
       <c r="B36" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>12</v>
@@ -1313,13 +1338,13 @@
       <c r="C39" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>2</v>
+      <c r="D39" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F39" s="17" t="s">
+      <c r="F39" s="14" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1327,13 +1352,13 @@
       <c r="A40" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="11" t="s">
+      <c r="B40" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E40" s="8" t="s">
@@ -1347,19 +1372,19 @@
       <c r="A41" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F41" s="12" t="s">
+      <c r="C41" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" s="17" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1396,7 +1421,7 @@
       <c r="D43" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F43" s="5" t="s">
@@ -1410,20 +1435,19 @@
       <c r="B44" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="12" t="s">
         <v>70</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="E44" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F44" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>3</v>
@@ -1431,13 +1455,13 @@
       <c r="B46" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E46" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F46" s="5" t="s">
@@ -1451,21 +1475,19 @@
       <c r="B47" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="12" t="s">
         <v>52</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E47" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F47" s="15" t="s">
+      <c r="F47" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>5</v>
@@ -1473,20 +1495,19 @@
       <c r="B50" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="12" t="s">
         <v>71</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E50" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="F50" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>6</v>
@@ -1494,22 +1515,19 @@
       <c r="B52" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="12" t="s">
         <v>72</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E52" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F52" s="15" t="s">
+      <c r="F52" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>12</v>
@@ -1520,13 +1538,13 @@
       <c r="C56" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>2</v>
+      <c r="D56" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="F56" s="14" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1534,19 +1552,19 @@
       <c r="A57" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B57" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D57" s="11" t="s">
+      <c r="B57" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F57" s="16">
+      <c r="F57" s="13">
         <v>44112</v>
       </c>
     </row>
@@ -1554,19 +1572,19 @@
       <c r="A58" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C58" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F58" s="12" t="s">
+      <c r="C58" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F58" s="17" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1603,13 +1621,13 @@
       <c r="D60" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E60" s="15" t="s">
+      <c r="E60" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I60" s="18"/>
+      <c r="I60" s="15"/>
     </row>
     <row r="61" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
@@ -1624,14 +1642,13 @@
       <c r="D61" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E61" s="15" t="s">
+      <c r="E61" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F61" s="15" t="s">
+      <c r="F61" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <v>3</v>
@@ -1639,16 +1656,16 @@
       <c r="B63" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C63" s="15" t="s">
+      <c r="C63" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E63" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F63" s="15"/>
+      <c r="E63" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F63" s="12"/>
     </row>
     <row r="64" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
@@ -1657,16 +1674,16 @@
       <c r="B64" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C64" s="15" t="s">
+      <c r="C64" s="12" t="s">
         <v>57</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E64" s="15" t="s">
+      <c r="E64" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F64" s="15" t="s">
+      <c r="F64" s="12" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1683,7 +1700,7 @@
       <c r="D65" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E65" s="15" t="s">
+      <c r="E65" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F65" s="5" t="s">
@@ -1697,21 +1714,19 @@
       <c r="B66" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C66" s="15" t="s">
+      <c r="C66" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E66" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F66" s="15" t="s">
+      <c r="E66" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F66" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>12</v>
@@ -1722,13 +1737,13 @@
       <c r="C69" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>2</v>
+      <c r="D69" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F69" s="17" t="s">
+      <c r="F69" s="14" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1736,19 +1751,19 @@
       <c r="A70" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B70" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D70" s="11" t="s">
+      <c r="B70" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F70" s="16">
+      <c r="F70" s="13">
         <v>44112</v>
       </c>
     </row>
@@ -1756,19 +1771,19 @@
       <c r="A71" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C71" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E71" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F71" s="12" t="s">
+      <c r="C71" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F71" s="17" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1805,7 +1820,7 @@
       <c r="D73" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E73" s="15" t="s">
+      <c r="E73" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F73" s="5" t="s">
@@ -1819,20 +1834,19 @@
       <c r="B74" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C74" s="15" t="s">
+      <c r="C74" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E74" s="15" t="s">
+      <c r="E74" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F74" s="15" t="s">
+      <c r="F74" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="76" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>3</v>
@@ -1840,20 +1854,19 @@
       <c r="B76" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C76" s="15" t="s">
+      <c r="C76" s="12" t="s">
         <v>76</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E76" s="15" t="s">
+      <c r="E76" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F76" s="15" t="s">
+      <c r="F76" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>4</v>
@@ -1861,13 +1874,13 @@
       <c r="B78" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C78" s="15" t="s">
+      <c r="C78" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E78" s="15" t="s">
+      <c r="E78" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F78" s="5" t="s">
@@ -1881,13 +1894,13 @@
       <c r="B79" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C79" s="15" t="s">
+      <c r="C79" s="12" t="s">
         <v>53</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E79" s="15" t="s">
+      <c r="E79" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F79" s="5" t="s">
@@ -1901,21 +1914,19 @@
       <c r="B80" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C80" s="15" t="s">
+      <c r="C80" s="12" t="s">
         <v>77</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E80" s="15" t="s">
+      <c r="E80" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F80" s="15" t="s">
+      <c r="F80" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="83" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>7</v>
@@ -1923,21 +1934,19 @@
       <c r="B83" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C83" s="15" t="s">
+      <c r="C83" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E83" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F83" s="15" t="s">
+      <c r="E83" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F83" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>12</v>
@@ -1948,13 +1957,13 @@
       <c r="C86" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>2</v>
+      <c r="D86" s="21" t="s">
+        <v>81</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F86" s="17" t="s">
+      <c r="F86" s="14" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1962,19 +1971,19 @@
       <c r="A87" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B87" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C87" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D87" s="11" t="s">
+      <c r="B87" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D87" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E87" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F87" s="16">
+      <c r="F87" s="13">
         <v>44112</v>
       </c>
     </row>
@@ -1982,19 +1991,19 @@
       <c r="A88" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B88" s="12" t="s">
+      <c r="B88" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C88" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D88" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E88" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F88" s="12" t="s">
+      <c r="C88" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E88" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F88" s="17" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2031,7 +2040,7 @@
       <c r="D90" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E90" s="15" t="s">
+      <c r="E90" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F90" s="5" t="s">
@@ -2045,13 +2054,13 @@
       <c r="B91" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C91" s="15" t="s">
+      <c r="C91" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E91" s="15" t="s">
+      <c r="E91" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F91" s="5" t="s">
@@ -2065,20 +2074,19 @@
       <c r="B92" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C92" s="15" t="s">
+      <c r="C92" s="12" t="s">
         <v>52</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E92" s="15" t="s">
+      <c r="E92" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F92" s="15" t="s">
+      <c r="F92" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="94" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>4</v>
@@ -2086,13 +2094,13 @@
       <c r="B94" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C94" s="15" t="s">
+      <c r="C94" s="12" t="s">
         <v>53</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E94" s="15" t="s">
+      <c r="E94" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F94" s="5" t="s">
@@ -2106,21 +2114,21 @@
       <c r="B95" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C95" s="15" t="s">
+      <c r="C95" s="12" t="s">
         <v>73</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E95" s="15" t="s">
+      <c r="E95" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F95" s="15" t="s">
+      <c r="F95" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D96" s="19"/>
+      <c r="D96" s="16"/>
     </row>
     <row r="97" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
@@ -2129,7 +2137,7 @@
       <c r="B97" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C97" s="15" t="s">
+      <c r="C97" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D97" s="6" t="s">
@@ -2138,12 +2146,10 @@
       <c r="E97" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F97" s="15" t="s">
+      <c r="F97" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>12</v>
@@ -2154,13 +2160,13 @@
       <c r="C100" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>2</v>
+      <c r="D100" s="21" t="s">
+        <v>82</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F100" s="17" t="s">
+      <c r="F100" s="14" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2168,19 +2174,19 @@
       <c r="A101" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B101" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C101" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D101" s="11" t="s">
+      <c r="B101" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C101" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" s="22" t="s">
         <v>2</v>
       </c>
       <c r="E101" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F101" s="16">
+      <c r="F101" s="13">
         <v>44112</v>
       </c>
     </row>
@@ -2188,19 +2194,19 @@
       <c r="A102" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B102" s="12" t="s">
+      <c r="B102" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C102" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D102" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E102" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F102" s="12" t="s">
+      <c r="C102" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D102" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E102" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F102" s="17" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2237,7 +2243,7 @@
       <c r="D104" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E104" s="15" t="s">
+      <c r="E104" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F104" s="5" t="s">
@@ -2251,13 +2257,13 @@
       <c r="B105" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C105" s="15" t="s">
+      <c r="C105" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E105" s="15" t="s">
+      <c r="E105" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F105" s="5" t="s">
@@ -2271,13 +2277,13 @@
       <c r="B106" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C106" s="15" t="s">
+      <c r="C106" s="12" t="s">
         <v>53</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E106" s="15" t="s">
+      <c r="E106" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F106" s="5" t="s">
@@ -2291,20 +2297,19 @@
       <c r="B107" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C107" s="15" t="s">
+      <c r="C107" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E107" s="15" t="s">
+      <c r="E107" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F107" s="15" t="s">
+      <c r="F107" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="109" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A109" s="9">
         <v>5</v>
@@ -2318,7 +2323,7 @@
       <c r="D109" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E109" s="15" t="s">
+      <c r="E109" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F109" s="5" t="s">
@@ -2332,13 +2337,13 @@
       <c r="B110" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C110" s="15" t="s">
+      <c r="C110" s="12" t="s">
         <v>68</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E110" s="15" t="s">
+      <c r="E110" s="12" t="s">
         <v>55</v>
       </c>
       <c r="F110" s="5" t="s">
@@ -2349,24 +2354,34 @@
       <c r="A111" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B111" s="12" t="s">
+      <c r="B111" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C111" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D111" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E111" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F111" s="12" t="s">
+      <c r="C111" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D111" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E111" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F111" s="17" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:F58"/>
     <mergeCell ref="B102:F102"/>
     <mergeCell ref="B111:F111"/>
     <mergeCell ref="B70:D70"/>
@@ -2374,16 +2389,6 @@
     <mergeCell ref="B87:D87"/>
     <mergeCell ref="B88:F88"/>
     <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>